<commit_message>
Update assurance case spreadsheet
</commit_message>
<xml_diff>
--- a/isolette/assurance-case/Isolette-Assurance-Case-Requirements-Outline.xlsx
+++ b/isolette/assurance-case/Isolette-Assurance-Case-Requirements-Outline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hatcliff/Dev/git-repos/INSPECTA-models-git/isolette/assurance-case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1580ECFA-DA27-BA4B-B3F3-96C10A14A802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB71A85D-B64C-2041-80BA-8574AB72456B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="760" windowWidth="28020" windowHeight="18040" activeTab="1" xr2:uid="{E1C3709C-219A-4F4F-AC32-BB0091E6CE70}"/>
+    <workbookView xWindow="800" yWindow="760" windowWidth="28600" windowHeight="18360" activeTab="1" xr2:uid="{E1C3709C-219A-4F4F-AC32-BB0091E6CE70}"/>
   </bookViews>
   <sheets>
     <sheet name="AC outline" sheetId="1" r:id="rId1"/>
@@ -1567,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5CB15B-FAF7-4B48-86C6-CA50B8A2EE9C}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1635,7 +1635,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="37"/>
     </row>
-    <row r="9" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>122</v>
       </c>
@@ -1916,7 +1916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD561E3-A00C-9741-852B-6653592B4264}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>